<commit_message>
Change design to use CAPD batch update-service job. Generate update-service.csv
</commit_message>
<xml_diff>
--- a/doc/account-changes-requested-KBOX-104070.xlsx
+++ b/doc/account-changes-requested-KBOX-104070.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pjansz\Documents\pd\sql\casa-11034\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pjansz\Documents\MyProjects\igt\pd\casa-11034\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -27,12 +27,6 @@
     <t>EmailVerified</t>
   </si>
   <si>
-    <t xml:space="preserve"> PP-Status</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> SecondChance-Status</t>
-  </si>
-  <si>
     <t xml:space="preserve"> PlayerID-Count</t>
   </si>
   <si>
@@ -54,10 +48,16 @@
     <t>Preactive</t>
   </si>
   <si>
-    <t>NewAccountStatus</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> New-EmailVerified2</t>
+    <t xml:space="preserve"> New-EmailVerified-state</t>
+  </si>
+  <si>
+    <t>NewAccount-state</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> SecondChance-state</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> PP-state</t>
   </si>
 </sst>
 </file>
@@ -612,10 +612,10 @@
   <tableColumns count="7">
     <tableColumn id="1" name="Scenario" dataDxfId="5"/>
     <tableColumn id="2" name="EmailVerified" dataDxfId="4"/>
-    <tableColumn id="4" name=" PP-Status" dataDxfId="3"/>
-    <tableColumn id="9" name=" SecondChance-Status" dataDxfId="1"/>
-    <tableColumn id="5" name="NewAccountStatus" dataDxfId="2"/>
-    <tableColumn id="11" name=" New-EmailVerified2" dataDxfId="0"/>
+    <tableColumn id="4" name=" PP-state" dataDxfId="3"/>
+    <tableColumn id="9" name=" SecondChance-state" dataDxfId="2"/>
+    <tableColumn id="5" name="NewAccount-state" dataDxfId="1"/>
+    <tableColumn id="11" name=" New-EmailVerified-state" dataDxfId="0"/>
     <tableColumn id="8" name=" PlayerID-Count"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -922,7 +922,7 @@
   <dimension ref="A1:G11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7:XFD7"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -931,7 +931,8 @@
     <col min="2" max="2" width="20.25" style="1" customWidth="1"/>
     <col min="3" max="3" width="21" style="1" customWidth="1"/>
     <col min="4" max="4" width="28.25" style="1" customWidth="1"/>
-    <col min="5" max="6" width="22.75" style="1" customWidth="1"/>
+    <col min="5" max="5" width="22.75" style="1" customWidth="1"/>
+    <col min="6" max="6" width="28.75" style="1" customWidth="1"/>
     <col min="7" max="7" width="19.625" customWidth="1"/>
   </cols>
   <sheetData>
@@ -943,19 +944,19 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="G1" t="s">
         <v>2</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="G1" t="s">
-        <v>4</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.2">
@@ -966,13 +967,13 @@
         <v>1</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="F2" s="1" t="b">
         <v>0</v>
@@ -989,13 +990,13 @@
         <v>1</v>
       </c>
       <c r="C3" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E3" s="1" t="s">
         <v>5</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>7</v>
       </c>
       <c r="F3" s="1" t="b">
         <v>1</v>
@@ -1012,13 +1013,13 @@
         <v>0</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="F4" s="1" t="b">
         <v>0</v>
@@ -1035,13 +1036,13 @@
         <v>1</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="D5" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E5" s="1" t="s">
         <v>5</v>
-      </c>
-      <c r="E5" s="1" t="s">
-        <v>7</v>
       </c>
       <c r="F5" s="1" t="b">
         <v>1</v>
@@ -1058,13 +1059,13 @@
         <v>1</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="F6" s="1" t="b">
         <v>0</v>
@@ -1081,13 +1082,13 @@
         <v>1</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="F7" s="1" t="b">
         <v>0</v>
@@ -1104,13 +1105,13 @@
         <v>1</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="F8" s="1" t="b">
         <v>0</v>
@@ -1127,13 +1128,13 @@
         <v>1</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="F9" s="1" t="b">
         <v>0</v>
@@ -1150,13 +1151,13 @@
         <v>0</v>
       </c>
       <c r="C10" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E10" s="1" t="s">
         <v>8</v>
-      </c>
-      <c r="D10" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="E10" s="1" t="s">
-        <v>10</v>
       </c>
       <c r="F10" s="1" t="b">
         <v>0</v>
@@ -1173,13 +1174,13 @@
         <v>1</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="F11" s="1" t="b">
         <v>0</v>

</xml_diff>

<commit_message>
Support revised scenarios, rules.
</commit_message>
<xml_diff>
--- a/doc/account-changes-requested-KBOX-104070.xlsx
+++ b/doc/account-changes-requested-KBOX-104070.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18431"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19126"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pjansz\Documents\Projects\igt\pd\casa-11034\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{40E6D818-F8AC-47B6-9D78-95C533FE6F6F}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12375"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12375" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="account-changes-requested-KBOX-" sheetId="1" r:id="rId1"/>
@@ -19,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="10">
   <si>
     <t>Scenario</t>
   </si>
@@ -54,8 +55,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="18" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -170,6 +171,13 @@
     <font>
       <sz val="11"/>
       <color theme="0"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <strike/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
@@ -515,11 +523,15 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -598,16 +610,16 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="A1:G11" totalsRowShown="0">
-  <autoFilter ref="A1:G11"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table2" displayName="Table2" ref="A1:G12" totalsRowShown="0">
+  <autoFilter ref="A1:G12" xr:uid="{00000000-0009-0000-0100-000002000000}"/>
   <tableColumns count="7">
-    <tableColumn id="1" name="Scenario" dataDxfId="5"/>
-    <tableColumn id="2" name="EmailVerified" dataDxfId="4"/>
-    <tableColumn id="4" name=" PP-state" dataDxfId="3"/>
-    <tableColumn id="9" name=" SecondChance-state" dataDxfId="2"/>
-    <tableColumn id="5" name="NewAccount-state" dataDxfId="1"/>
-    <tableColumn id="11" name=" New-EmailVerified-state" dataDxfId="0"/>
-    <tableColumn id="8" name=" PlayerID-Count"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Scenario" dataDxfId="5"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="EmailVerified" dataDxfId="4"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name=" PP-state" dataDxfId="3"/>
+    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0000-000009000000}" name=" SecondChance-state" dataDxfId="2"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="NewAccount-state" dataDxfId="1"/>
+    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0000-00000B000000}" name=" New-EmailVerified-state" dataDxfId="0"/>
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" name=" PlayerID-Count"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -909,11 +921,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G11"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:G12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="A12" sqref="A12:XFD12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -967,7 +979,7 @@
         <v>5</v>
       </c>
       <c r="F2" s="1" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G2">
         <v>905160</v>
@@ -1010,7 +1022,7 @@
         <v>3</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="F4" s="1" t="b">
         <v>0</v>
@@ -1059,7 +1071,7 @@
         <v>5</v>
       </c>
       <c r="F6" s="1" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G6">
         <v>3</v>
@@ -1082,7 +1094,7 @@
         <v>5</v>
       </c>
       <c r="F7" s="1" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G7">
         <v>2</v>
@@ -1105,7 +1117,7 @@
         <v>5</v>
       </c>
       <c r="F8" s="1" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G8">
         <v>1</v>
@@ -1128,7 +1140,7 @@
         <v>5</v>
       </c>
       <c r="F9" s="1" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G9">
         <v>2</v>
@@ -1157,33 +1169,57 @@
         <v>1450</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A11" s="1">
+    <row r="11" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A11" s="2">
         <v>10</v>
       </c>
-      <c r="B11" s="1" t="b">
-        <v>1</v>
-      </c>
-      <c r="C11" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="D11" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="E11" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="F11" s="1" t="b">
+      <c r="B11" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="E11" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="F11" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="G11" s="3">
+        <v>98228</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A12" s="1">
+        <v>11</v>
+      </c>
+      <c r="B12" s="1" t="b">
         <v>0</v>
       </c>
-      <c r="G11">
-        <v>98228</v>
+      <c r="C12" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F12" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="G12">
+        <v>8471</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
   <tableParts count="1">
-    <tablePart r:id="rId1"/>
+    <tablePart r:id="rId2"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>